<commit_message>
Including new fields to the view's list
</commit_message>
<xml_diff>
--- a/SharePoint/sample.xlsx
+++ b/SharePoint/sample.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="68">
   <si>
     <t xml:space="preserve">Métadonnées</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">Plusieurs lignes de texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mots clés</t>
   </si>
   <si>
     <t xml:space="preserve">* Voir onglet suivant (Domaine de valeurs) pour les détails.</t>
@@ -713,7 +716,7 @@
   <dimension ref="A1:P1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -816,7 +819,7 @@
       </c>
       <c r="H4" s="13"/>
       <c r="I4" s="13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4" s="13" t="n">
         <v>2</v>
@@ -843,10 +846,10 @@
       <c r="G5" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="H5" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14" t="n">
+        <v>4</v>
+      </c>
       <c r="J5" s="14" t="n">
         <v>1</v>
       </c>
@@ -873,9 +876,11 @@
         <v>1</v>
       </c>
       <c r="H6" s="14" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" s="14"/>
+        <v>1</v>
+      </c>
+      <c r="I6" s="14" t="n">
+        <v>3</v>
+      </c>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
@@ -887,14 +892,22 @@
         <f aca="false">IFERROR(VLOOKUP(C7,Types,2,0),"")</f>
         <v/>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
+      <c r="G7" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="H7" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="14" t="n">
+        <v>1</v>
+      </c>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
@@ -1739,7 +1752,7 @@
     </row>
     <row r="52" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="18"/>
@@ -1756,7 +1769,7 @@
     </row>
     <row r="53" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C53" s="19"/>
       <c r="D53" s="19"/>
@@ -1773,7 +1786,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C54" s="20"/>
       <c r="D54" s="20"/>
@@ -1875,7 +1888,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.12"/>
@@ -1887,10 +1900,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="23"/>
@@ -2293,7 +2306,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.14"/>
@@ -2301,21 +2314,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>6</v>
@@ -2323,10 +2336,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>15</v>
@@ -2334,10 +2347,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>4</v>
@@ -2345,10 +2358,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>10</v>
@@ -2356,10 +2369,10 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>11</v>
@@ -2367,10 +2380,10 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>9</v>
@@ -2378,10 +2391,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>8</v>
@@ -2392,7 +2405,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>20</v>
@@ -2403,7 +2416,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>3</v>
@@ -2411,10 +2424,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>7</v>
@@ -2425,7 +2438,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>2</v>
@@ -2433,10 +2446,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>17</v>
@@ -2444,7 +2457,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>29</v>
@@ -2452,7 +2465,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>19</v>
@@ -2460,7 +2473,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>12</v>
@@ -2468,7 +2481,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>25</v>
@@ -2476,7 +2489,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>5</v>
@@ -2484,7 +2497,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>22</v>
@@ -2492,7 +2505,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>24</v>
@@ -2500,7 +2513,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>18</v>
@@ -2508,7 +2521,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>31</v>
@@ -2516,7 +2529,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>16</v>
@@ -2524,7 +2537,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>14</v>
@@ -2532,7 +2545,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>1</v>
@@ -2540,7 +2553,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>0</v>
@@ -2548,7 +2561,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>33</v>
@@ -2556,7 +2569,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>23</v>
@@ -2564,7 +2577,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>32</v>
@@ -2572,7 +2585,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>26</v>
@@ -2580,7 +2593,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>21</v>
@@ -2588,7 +2601,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>27</v>
@@ -2596,7 +2609,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>13</v>
@@ -2604,7 +2617,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>30</v>
@@ -2612,7 +2625,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>28</v>

</xml_diff>